<commit_message>
update home dan spp
</commit_message>
<xml_diff>
--- a/Notulen 22 Juni 2015.xlsx
+++ b/Notulen 22 Juni 2015.xlsx
@@ -24,9 +24,6 @@
     <t>Field yang harus ada pada upload stock via excel utamakan yang wajib dalam tabel</t>
   </si>
   <si>
-    <t>Pada text area alamat kasih keterangan 160 karakter</t>
-  </si>
-  <si>
     <t>tanggal SPP tidak bisa dirubah</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>nilai rencana bayar di cetak spp belum masuk</t>
+  </si>
+  <si>
+    <t>Pada text area alamat kasih keterangan 100 karakter</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J1" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
@@ -602,13 +602,13 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -616,12 +616,12 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -629,12 +629,12 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -642,12 +642,12 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -655,12 +655,12 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -668,15 +668,15 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="3"/>
@@ -692,158 +692,158 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -851,11 +851,11 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L21" s="3"/>
     </row>
@@ -864,10 +864,10 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -877,10 +877,10 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -890,12 +890,12 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -903,10 +903,10 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -916,10 +916,10 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -931,7 +931,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="3"/>
@@ -942,12 +942,12 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -955,12 +955,12 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -968,12 +968,12 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -981,12 +981,12 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -994,12 +994,12 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1007,12 +1007,12 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -1020,12 +1020,12 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="3"/>
@@ -1046,12 +1046,12 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -1059,12 +1059,12 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -1072,11 +1072,11 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L40" s="3"/>
     </row>
@@ -1085,12 +1085,12 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -1098,12 +1098,12 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="3"/>
@@ -1124,10 +1124,10 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
@@ -1137,10 +1137,10 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
@@ -1150,10 +1150,10 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="3"/>
@@ -1176,11 +1176,11 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L50" s="3"/>
     </row>
@@ -1197,7 +1197,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1207,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K1" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="K3" s="3"/>
       <c r="M3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1234,10 +1234,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M4" s="3"/>
     </row>
@@ -1246,10 +1246,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M5" s="3"/>
     </row>
@@ -1258,10 +1258,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -1270,10 +1270,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M7" s="3"/>
     </row>
@@ -1282,10 +1282,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M8" s="3"/>
     </row>
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K9" s="3"/>
       <c r="M9" s="3"/>
@@ -1304,10 +1304,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M10" s="3"/>
     </row>
@@ -1316,10 +1316,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M11" s="3"/>
     </row>

</xml_diff>